<commit_message>
Crops with State and Districts.
</commit_message>
<xml_diff>
--- a/ML/Data/Plants_and_Districts.xlsx
+++ b/ML/Data/Plants_and_Districts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Cultivo\ML\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D4BBC4-894E-4DF7-8755-EC2F0CE6E261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5B4CF0-B28A-40FE-A077-A919A80F94AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2475" yWindow="2745" windowWidth="20490" windowHeight="5400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2745" windowWidth="20490" windowHeight="5400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="187">
   <si>
     <t>crop</t>
   </si>
@@ -39,9 +39,6 @@
     <t>rice</t>
   </si>
   <si>
-    <t>westbengal</t>
-  </si>
-  <si>
     <t>medinipur</t>
   </si>
   <si>
@@ -445,6 +442,150 @@
   </si>
   <si>
     <t>utharakhand</t>
+  </si>
+  <si>
+    <t>gwalior</t>
+  </si>
+  <si>
+    <t>morena</t>
+  </si>
+  <si>
+    <t>shoipur</t>
+  </si>
+  <si>
+    <t>bhind</t>
+  </si>
+  <si>
+    <t>hosangabad</t>
+  </si>
+  <si>
+    <t>harda</t>
+  </si>
+  <si>
+    <t>balaghat</t>
+  </si>
+  <si>
+    <t>datia</t>
+  </si>
+  <si>
+    <t>shivpuri</t>
+  </si>
+  <si>
+    <t>narsinghpur</t>
+  </si>
+  <si>
+    <t>seoni</t>
+  </si>
+  <si>
+    <t>betul</t>
+  </si>
+  <si>
+    <t>tickmagarh</t>
+  </si>
+  <si>
+    <t>guna</t>
+  </si>
+  <si>
+    <t>janbalpur</t>
+  </si>
+  <si>
+    <t>khandwa</t>
+  </si>
+  <si>
+    <t>rice', 'maize', 'chickpea', 'kidneybeans', 'pigeonpeas', 'mothbeans', 'mungbean', 'blackgram', 'lentil', 'pomegranate', 'banana', 'mango', 'grapes', 'watermelon', 'muskmelon', 'apple', 'orange', 'papaya', 'coconut', 'cotton', 'jute', 'coffee']</t>
+  </si>
+  <si>
+    <t>kerala</t>
+  </si>
+  <si>
+    <t>palakkad</t>
+  </si>
+  <si>
+    <t>alappuzha</t>
+  </si>
+  <si>
+    <t>kottayam</t>
+  </si>
+  <si>
+    <t>thrissur</t>
+  </si>
+  <si>
+    <t>malappuram</t>
+  </si>
+  <si>
+    <t>wayanad</t>
+  </si>
+  <si>
+    <t>ernakulam</t>
+  </si>
+  <si>
+    <t>tripura</t>
+  </si>
+  <si>
+    <t>west tripura</t>
+  </si>
+  <si>
+    <t>south tripura</t>
+  </si>
+  <si>
+    <t>dhalia</t>
+  </si>
+  <si>
+    <t>manipur</t>
+  </si>
+  <si>
+    <t>Imphal</t>
+  </si>
+  <si>
+    <t>Thoubal</t>
+  </si>
+  <si>
+    <t>Bishnupur</t>
+  </si>
+  <si>
+    <t>arunachal pradesh</t>
+  </si>
+  <si>
+    <t>tawang</t>
+  </si>
+  <si>
+    <t>dirang</t>
+  </si>
+  <si>
+    <t>bomdila</t>
+  </si>
+  <si>
+    <t>shegaon</t>
+  </si>
+  <si>
+    <t>west kameng</t>
+  </si>
+  <si>
+    <t>dibang</t>
+  </si>
+  <si>
+    <t>lohit</t>
+  </si>
+  <si>
+    <t>changyak</t>
+  </si>
+  <si>
+    <t>naga</t>
+  </si>
+  <si>
+    <t>maize</t>
+  </si>
+  <si>
+    <t>chindwaara</t>
+  </si>
+  <si>
+    <t>khargone</t>
+  </si>
+  <si>
+    <t>bharwani</t>
+  </si>
+  <si>
+    <t>west bengal</t>
   </si>
 </sst>
 </file>
@@ -762,20 +903,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C123"/>
+  <dimension ref="A1:F163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="B113" sqref="B113"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -786,662 +927,887 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" t="s">
         <v>45</v>
-      </c>
-      <c r="C41" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
+        <v>60</v>
+      </c>
+      <c r="C56" t="s">
         <v>61</v>
-      </c>
-      <c r="C56" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
+        <v>71</v>
+      </c>
+      <c r="C66" t="s">
         <v>72</v>
-      </c>
-      <c r="C66" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C69" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C74" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C75" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C76" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
+        <v>83</v>
+      </c>
+      <c r="C77" t="s">
         <v>84</v>
-      </c>
-      <c r="C77" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C80" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C82" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
+        <v>90</v>
+      </c>
+      <c r="C83" t="s">
         <v>91</v>
-      </c>
-      <c r="C83" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C84" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C85" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C86" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C88" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C89" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
+        <v>98</v>
+      </c>
+      <c r="C90" t="s">
         <v>99</v>
-      </c>
-      <c r="C90" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C91" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C92" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C93" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C94" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C95" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C96" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C97" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C98" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
+        <v>108</v>
+      </c>
+      <c r="C99" t="s">
         <v>109</v>
-      </c>
-      <c r="C99" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C100" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C101" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C102" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C103" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C104" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
+        <v>115</v>
+      </c>
+      <c r="C105" t="s">
         <v>116</v>
-      </c>
-      <c r="C105" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C106" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C107" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C108" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C109" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C110" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C111" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C112" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
+        <v>124</v>
+      </c>
+      <c r="C113" t="s">
         <v>125</v>
-      </c>
-      <c r="C113" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C114" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C115" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C116" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C117" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
+        <v>130</v>
+      </c>
+      <c r="C118" t="s">
         <v>131</v>
-      </c>
-      <c r="C118" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C119" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C120" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C121" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C122" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="123" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>137</v>
+        <v>136</v>
+      </c>
+      <c r="C123" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C124" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C125" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C126" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C127" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C128" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C129" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C130" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C131" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C132" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C133" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C134" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C135" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="136" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C136" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="137" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C137" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="138" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C138" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="139" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B139" t="s">
+        <v>156</v>
+      </c>
+      <c r="C139" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="140" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C140" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="141" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C141" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C142" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="143" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C143" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C144" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C145" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B146" t="s">
+        <v>164</v>
+      </c>
+      <c r="C146" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="147" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C147" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="148" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C148" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="149" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B149" t="s">
+        <v>168</v>
+      </c>
+      <c r="C149" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="150" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C150" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="151" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C151" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="152" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B152" t="s">
+        <v>172</v>
+      </c>
+      <c r="C152" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="153" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C153" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="154" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C154" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="155" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C155" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="156" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C156" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="157" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C157" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="158" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C158" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="159" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C159" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="160" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C160" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>182</v>
+      </c>
+      <c r="B161" t="s">
+        <v>136</v>
+      </c>
+      <c r="C161" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C162" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C163" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Crops with Districts Update
</commit_message>
<xml_diff>
--- a/ML/Data/Plants_and_Districts.xlsx
+++ b/ML/Data/Plants_and_Districts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Cultivo\ML\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7255DA08-914B-4172-A43F-D49CB6A69E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A01ACA0-A1EA-4635-9139-2FD0FEB50C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2745" windowWidth="20490" windowHeight="5400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="241">
   <si>
     <t>crop</t>
   </si>
@@ -492,9 +492,6 @@
     <t>khandwa</t>
   </si>
   <si>
-    <t>rice', 'maize', 'chickpea', 'kidneybeans', 'pigeonpeas', 'mothbeans', 'mungbean', 'blackgram', 'lentil', 'pomegranate', 'banana', 'mango', 'grapes', 'watermelon', 'muskmelon', 'apple', 'orange', 'papaya', 'coconut', 'cotton', 'jute', 'coffee']</t>
-  </si>
-  <si>
     <t>kerala</t>
   </si>
   <si>
@@ -586,6 +583,171 @@
   </si>
   <si>
     <t>west bengal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          </t>
+  </si>
+  <si>
+    <t>chickpea', 'kidneybeans', 'pigeonpeas', 'mothbeans', 'mungbean', 'blackgram', 'lentil', 'pomegranate', 'banana', 'mango', 'grapes', 'watermelon', 'muskmelon', 'apple', 'orange', 'papaya', 'coconut', 'cotton', 'jute', 'coffee']</t>
+  </si>
+  <si>
+    <t>vizianagaram</t>
+  </si>
+  <si>
+    <t>kurnool</t>
+  </si>
+  <si>
+    <t>kadapa</t>
+  </si>
+  <si>
+    <t>koppal</t>
+  </si>
+  <si>
+    <t>devanagere</t>
+  </si>
+  <si>
+    <t>haveri</t>
+  </si>
+  <si>
+    <t>belgavi</t>
+  </si>
+  <si>
+    <t>chikkaballapur</t>
+  </si>
+  <si>
+    <t>chikmangalur</t>
+  </si>
+  <si>
+    <t>chitradurga</t>
+  </si>
+  <si>
+    <t>gadag</t>
+  </si>
+  <si>
+    <t>rajasthan</t>
+  </si>
+  <si>
+    <t>bhilwara</t>
+  </si>
+  <si>
+    <t>chittorgarh</t>
+  </si>
+  <si>
+    <t>udaipur</t>
+  </si>
+  <si>
+    <t>banswara</t>
+  </si>
+  <si>
+    <t>bundi</t>
+  </si>
+  <si>
+    <t>rajasmand</t>
+  </si>
+  <si>
+    <t>dungarpur</t>
+  </si>
+  <si>
+    <t>nashik</t>
+  </si>
+  <si>
+    <t>pune</t>
+  </si>
+  <si>
+    <t>solapur</t>
+  </si>
+  <si>
+    <t>Ahmednagar</t>
+  </si>
+  <si>
+    <t>buldana</t>
+  </si>
+  <si>
+    <t>Sangli</t>
+  </si>
+  <si>
+    <t>jalna</t>
+  </si>
+  <si>
+    <t>dhule</t>
+  </si>
+  <si>
+    <t>satara</t>
+  </si>
+  <si>
+    <t>kishanganj</t>
+  </si>
+  <si>
+    <t>araria</t>
+  </si>
+  <si>
+    <t>katihar</t>
+  </si>
+  <si>
+    <t>madhepura</t>
+  </si>
+  <si>
+    <t>saharsa</t>
+  </si>
+  <si>
+    <t>supaul</t>
+  </si>
+  <si>
+    <t>khagaria</t>
+  </si>
+  <si>
+    <t>muzzaffarpur</t>
+  </si>
+  <si>
+    <t>vaishali</t>
+  </si>
+  <si>
+    <t>begusarayi</t>
+  </si>
+  <si>
+    <t>meerut</t>
+  </si>
+  <si>
+    <t>ghaziabad</t>
+  </si>
+  <si>
+    <t>bulandshahr</t>
+  </si>
+  <si>
+    <t>farrukhabad</t>
+  </si>
+  <si>
+    <t>gonda</t>
+  </si>
+  <si>
+    <t>jaunpur</t>
+  </si>
+  <si>
+    <t>etah</t>
+  </si>
+  <si>
+    <t>firozabad</t>
+  </si>
+  <si>
+    <t>manipuri</t>
+  </si>
+  <si>
+    <t>varnasi</t>
+  </si>
+  <si>
+    <t>himachal pradesh</t>
+  </si>
+  <si>
+    <t>mandi</t>
+  </si>
+  <si>
+    <t>kangra</t>
+  </si>
+  <si>
+    <t>hamirpur</t>
+  </si>
+  <si>
+    <t>chamba</t>
   </si>
 </sst>
 </file>
@@ -621,8 +783,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -903,10 +1066,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F163"/>
+  <dimension ref="A1:F222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="C164" sqref="C164"/>
+    <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
+      <selection activeCell="C223" sqref="C223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,19 +1095,22 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
-        <v>155</v>
+      <c r="F2" s="1" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>5</v>
       </c>
+      <c r="F3" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
@@ -1665,145 +1831,461 @@
     </row>
     <row r="139" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
+        <v>155</v>
+      </c>
+      <c r="C139" t="s">
         <v>156</v>
-      </c>
-      <c r="C139" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="140" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C140" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="141" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C141" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="142" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C142" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="143" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C143" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="144" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C144" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="145" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C145" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="146" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
+        <v>163</v>
+      </c>
+      <c r="C146" t="s">
         <v>164</v>
-      </c>
-      <c r="C146" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="147" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C147" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="148" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C148" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="149" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
+        <v>167</v>
+      </c>
+      <c r="C149" t="s">
         <v>168</v>
-      </c>
-      <c r="C149" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="150" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C150" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="151" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C151" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="152" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
+        <v>171</v>
+      </c>
+      <c r="C152" t="s">
         <v>172</v>
-      </c>
-      <c r="C152" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="153" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C153" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="154" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C154" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="155" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C155" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="156" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C156" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="157" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C157" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="158" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C158" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="159" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C159" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="160" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C160" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B161" t="s">
         <v>136</v>
       </c>
       <c r="C161" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C162" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C163" t="s">
-        <v>185</v>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B164" t="s">
+        <v>44</v>
+      </c>
+      <c r="C164" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C165" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C166" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C167" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C168" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C169" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B170" t="s">
+        <v>115</v>
+      </c>
+      <c r="C170" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C171" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C172" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C173" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C174" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C175" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C176" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="177" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C177" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="178" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C178" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="179" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C179" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="180" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B180" t="s">
+        <v>199</v>
+      </c>
+      <c r="C180" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="181" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C181" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="182" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C182" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="183" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C183" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="184" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C184" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="185" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C185" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="186" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C186" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="187" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B187" t="s">
+        <v>130</v>
+      </c>
+      <c r="C187" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="188" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C188" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="189" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C189" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="190" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C190" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="191" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C191" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="192" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C192" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="193" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C193" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="194" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C194" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="195" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C195" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="196" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C196" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="197" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B197" t="s">
+        <v>71</v>
+      </c>
+      <c r="C197" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="198" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C198" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="199" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C199" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="200" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C200" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="201" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C201" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="202" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C202" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="203" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C203" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="204" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C204" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="205" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C205" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="206" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C206" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="207" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C207" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="208" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B208" t="s">
+        <v>137</v>
+      </c>
+      <c r="C208" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="209" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C209" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="210" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C210" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="211" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C211" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="212" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C212" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="213" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C213" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="214" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C214" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="215" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C215" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="216" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C216" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="217" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C217" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="218" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B218" t="s">
+        <v>236</v>
+      </c>
+      <c r="C218" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="219" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C219" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="220" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C220" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="221" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C221" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="222" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C222" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>